<commit_message>
Added Frame work Annotations, Handled Exceptions ,Added Retry Listener, Removed unused code
Added Frame work Annotations
Handled Exceptions
Added Retry Listener
Removed unused code
</commit_message>
<xml_diff>
--- a/WebAutomationFramework/src/test/resources/excel/TestData.xlsx
+++ b/WebAutomationFramework/src/test/resources/excel/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>First Name</t>
   </si>
@@ -110,7 +110,10 @@
     <t>admin1234</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,25 +514,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -543,28 +546,31 @@
         <v>22</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -577,8 +583,8 @@
       <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>25</v>
+      <c r="E2" t="s">
+        <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>25</v>
@@ -598,13 +604,16 @@
       <c r="K2" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -613,28 +622,31 @@
         <v>24</v>
       </c>
       <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -648,33 +660,36 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
@@ -682,8 +697,8 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>25</v>
+      <c r="E5" t="s">
+        <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>25</v>
@@ -701,6 +716,9 @@
         <v>25</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Edit for Remote Execution
Driver Factory
To support remote mode for docker
</commit_message>
<xml_diff>
--- a/WebAutomationFramework/src/test/resources/excel/TestData.xlsx
+++ b/WebAutomationFramework/src/test/resources/excel/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>First Name</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>BrowserVersion</t>
+  </si>
+  <si>
+    <t>99.0.4844.51</t>
   </si>
 </sst>
 </file>
@@ -514,25 +520,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -549,28 +556,31 @@
         <v>31</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -587,7 +597,7 @@
         <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>25</v>
@@ -607,8 +617,11 @@
       <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -624,29 +637,32 @@
       <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -662,29 +678,32 @@
       <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -701,7 +720,7 @@
         <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>25</v>
@@ -719,6 +738,9 @@
         <v>25</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docker file , code refactor , elastic search class for dashboard
</commit_message>
<xml_diff>
--- a/WebAutomationFramework/src/test/resources/excel/TestData.xlsx
+++ b/WebAutomationFramework/src/test/resources/excel/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="37">
   <si>
     <t>First Name</t>
   </si>
@@ -119,7 +119,13 @@
     <t>BrowserVersion</t>
   </si>
   <si>
-    <t>99.0.4844.51</t>
+    <t>94.0.4606.61</t>
+  </si>
+  <si>
+    <t>92.0.1</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -520,10 +526,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -744,6 +750,88 @@
         <v>25</v>
       </c>
     </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>